<commit_message>
scrum and diary updatet
</commit_message>
<xml_diff>
--- a/doc/Task10/scrum_v01.xlsx
+++ b/doc/Task10/scrum_v01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18680" windowHeight="6330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4452" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
+  <oleSize ref="A2:M9"/>
 </workbook>
 </file>
 
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,13 +627,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -649,7 +649,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -657,7 +657,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -665,7 +665,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -673,7 +673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -690,23 +690,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6328125" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -732,7 +732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -756,7 +756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -780,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -803,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>33</v>
       </c>
@@ -812,32 +812,32 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
@@ -851,27 +851,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" customWidth="1"/>
-    <col min="3" max="3" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.36328125" customWidth="1"/>
-    <col min="9" max="9" width="7.90625" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" customWidth="1"/>
-    <col min="11" max="11" width="7.36328125" customWidth="1"/>
-    <col min="12" max="12" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -909,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -946,7 +945,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1.2</v>
       </c>
@@ -985,7 +984,7 @@
       </c>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -1024,7 +1023,7 @@
       </c>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -1063,7 +1062,7 @@
       </c>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>1.4</v>
       </c>
@@ -1095,14 +1094,14 @@
         <v>4</v>
       </c>
       <c r="K6" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L6" t="s">
         <v>63</v>
       </c>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>1.5</v>
       </c>
@@ -1141,7 +1140,7 @@
       </c>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>1.6</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>1.7</v>
       </c>
@@ -1217,12 +1216,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H11" s="9" t="s">
         <v>48</v>
       </c>
@@ -1236,15 +1235,15 @@
       </c>
       <c r="K11">
         <f>SUM(K2:K9)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:13" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:13" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:13" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1258,14 +1257,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>